<commit_message>
updated PEEK groups in saftgamma_database.xml in sgtpy package.
</commit_message>
<xml_diff>
--- a/sgtpy_NETGP/database/saftgamma_database.xlsx
+++ b/sgtpy_NETGP/database/saftgamma_database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn621\Anaconda3\Lib\site-packages\sgtpy_NETGP\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn621\Anaconda3\envs\py397\Lib\site-packages\sgtpy_NETGP\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F40BA890-6E69-4C72-9CD3-AF384BC31B18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E4272F01-2405-41FC-863B-DBC401180049}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="94">
   <si>
     <t>vk*</t>
   </si>
@@ -304,6 +304,9 @@
   <si>
     <t>aCH_PS</t>
   </si>
+  <si>
+    <t>aCOaC</t>
+  </si>
 </sst>
 </file>
 
@@ -382,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -394,6 +397,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -733,10 +740,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3211,83 +3221,83 @@
         <v>52.031100000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57">
+    <row r="57" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>6.0316619697112099E-2</v>
+      </c>
+      <c r="D57" s="2">
+        <v>7.7302521096828096</v>
+      </c>
+      <c r="E57" s="2">
+        <v>514.58333405805604</v>
+      </c>
+      <c r="F57" s="2">
+        <v>8</v>
+      </c>
+      <c r="G57" s="2">
+        <v>6</v>
+      </c>
+      <c r="H57" s="2">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2">
         <v>2</v>
       </c>
-      <c r="C57">
-        <v>0.65529999999999999</v>
-      </c>
-      <c r="D57">
-        <v>3.3942000000000001</v>
-      </c>
-      <c r="E57">
-        <v>313.35000000000002</v>
-      </c>
-      <c r="F57">
-        <v>8</v>
-      </c>
-      <c r="G57">
-        <v>6</v>
-      </c>
-      <c r="H57">
-        <v>3</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="J57">
-        <v>2</v>
-      </c>
-      <c r="K57">
-        <v>2</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
-      </c>
-      <c r="N57">
-        <v>57.027240000000013</v>
+      <c r="K57" s="2">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2">
+        <v>0</v>
+      </c>
+      <c r="N57" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>0.54262999999999995</v>
+        <v>0.65529999999999999</v>
       </c>
       <c r="D58">
-        <v>3.3218000000000001</v>
+        <v>3.3942000000000001</v>
       </c>
       <c r="E58">
-        <v>303.35000000000002</v>
+        <v>313.35000000000002</v>
       </c>
       <c r="F58">
-        <v>8.2760999999999996</v>
+        <v>8</v>
       </c>
       <c r="G58">
         <v>6</v>
       </c>
       <c r="H58">
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
         <v>2</v>
       </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="J58">
-        <v>1</v>
-      </c>
       <c r="K58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -3296,39 +3306,39 @@
         <v>0</v>
       </c>
       <c r="N58">
-        <v>39.035939999999997</v>
+        <v>57.027240000000013</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>0.54684999999999995</v>
+        <v>0.54262999999999995</v>
       </c>
       <c r="D59">
-        <v>3.9112</v>
+        <v>3.3218000000000001</v>
       </c>
       <c r="E59">
-        <v>525.22</v>
+        <v>303.35000000000002</v>
       </c>
       <c r="F59">
-        <v>19.05</v>
+        <v>8.2760999999999996</v>
       </c>
       <c r="G59">
         <v>6</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -3340,39 +3350,39 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>43.04392</v>
+        <v>39.035939999999997</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>0.40981000000000001</v>
+        <v>0.54684999999999995</v>
       </c>
       <c r="D60">
-        <v>2.8565999999999998</v>
+        <v>3.9112</v>
       </c>
       <c r="E60">
-        <v>330.18</v>
+        <v>525.22</v>
       </c>
       <c r="F60">
-        <v>10.127000000000001</v>
+        <v>19.05</v>
       </c>
       <c r="G60">
         <v>6</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -3384,12 +3394,12 @@
         <v>0</v>
       </c>
       <c r="N60">
-        <v>45.059600000000003</v>
+        <v>43.04392</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -3401,7 +3411,7 @@
         <v>2.8565999999999998</v>
       </c>
       <c r="E61">
-        <v>248.2</v>
+        <v>330.18</v>
       </c>
       <c r="F61">
         <v>10.127000000000001</v>
@@ -3428,6 +3438,50 @@
         <v>0</v>
       </c>
       <c r="N61">
+        <v>45.059600000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0.40981000000000001</v>
+      </c>
+      <c r="D62">
+        <v>2.8565999999999998</v>
+      </c>
+      <c r="E62">
+        <v>248.2</v>
+      </c>
+      <c r="F62">
+        <v>10.127000000000001</v>
+      </c>
+      <c r="G62">
+        <v>6</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
         <v>44.051760000000002</v>
       </c>
     </row>
@@ -3438,11 +3492,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E363"/>
+  <dimension ref="A1:E364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D272" sqref="D272"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5153,29 +5207,28 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C122" s="4">
-        <v>416.69</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E122" s="6"/>
+      <c r="A122" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C122" s="2">
+        <v>683.29988702381002</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C123" s="4">
-        <v>429.16</v>
+        <v>416.69</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>76</v>
@@ -5187,13 +5240,13 @@
         <v>92</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C124" s="4">
-        <v>331.61</v>
-      </c>
-      <c r="D124" s="4">
-        <v>9.0686999999999998</v>
+        <v>429.16</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E124" s="6"/>
     </row>
@@ -5202,13 +5255,13 @@
         <v>92</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C125" s="4">
-        <v>333.11</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>76</v>
+        <v>331.61</v>
+      </c>
+      <c r="D125" s="4">
+        <v>9.0686999999999998</v>
       </c>
       <c r="E125" s="6"/>
     </row>
@@ -5217,13 +5270,13 @@
         <v>92</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C126" s="4">
-        <v>357.78</v>
-      </c>
-      <c r="D126" s="4">
-        <v>38.64</v>
+        <v>333.11</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E126" s="6"/>
     </row>
@@ -5232,13 +5285,13 @@
         <v>92</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C127" s="4">
-        <v>386.05</v>
-      </c>
-      <c r="D127" s="4" t="s">
-        <v>76</v>
+        <v>357.78</v>
+      </c>
+      <c r="D127" s="4">
+        <v>38.64</v>
       </c>
       <c r="E127" s="6"/>
     </row>
@@ -5247,10 +5300,10 @@
         <v>92</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C128" s="4">
-        <v>512.16</v>
+        <v>386.05</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>76</v>
@@ -5262,10 +5315,10 @@
         <v>92</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C129" s="4">
-        <v>471.23</v>
+        <v>512.16</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>76</v>
@@ -5277,10 +5330,10 @@
         <v>92</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C130" s="4">
-        <v>448.75</v>
+        <v>471.23</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>76</v>
@@ -5292,10 +5345,10 @@
         <v>92</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>76</v>
+        <v>41</v>
+      </c>
+      <c r="C131" s="4">
+        <v>448.75</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>76</v>
@@ -5307,13 +5360,13 @@
         <v>92</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C132" s="4">
-        <v>331.61</v>
-      </c>
-      <c r="D132" s="4">
-        <v>9.0686999999999998</v>
+        <v>45</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E132" s="6"/>
     </row>
@@ -5322,13 +5375,13 @@
         <v>92</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C133" s="4">
-        <v>340.7</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>76</v>
+        <v>331.61</v>
+      </c>
+      <c r="D133" s="4">
+        <v>9.0686999999999998</v>
       </c>
       <c r="E133" s="6"/>
     </row>
@@ -5337,10 +5390,10 @@
         <v>92</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C134" s="4">
-        <v>549.72</v>
+        <v>340.7</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>76</v>
@@ -5352,39 +5405,40 @@
         <v>92</v>
       </c>
       <c r="B135" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C135" s="4">
+        <v>549.72</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E135" s="6"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C136" s="4">
         <v>426.72</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <v>18.03</v>
       </c>
-      <c r="E135" s="6"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>19</v>
-      </c>
-      <c r="B136" t="s">
-        <v>20</v>
-      </c>
-      <c r="C136">
-        <v>462.04</v>
-      </c>
-      <c r="D136" t="s">
-        <v>76</v>
-      </c>
+      <c r="E136" s="6"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C137">
-        <v>473.66</v>
+        <v>462.04</v>
       </c>
       <c r="D137" t="s">
         <v>76</v>
@@ -5395,10 +5449,10 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C138">
-        <v>394.83</v>
+        <v>473.66</v>
       </c>
       <c r="D138" t="s">
         <v>76</v>
@@ -5409,10 +5463,10 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C139">
-        <v>329.03</v>
+        <v>394.83</v>
       </c>
       <c r="D139" t="s">
         <v>76</v>
@@ -5423,10 +5477,10 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C140">
-        <v>434.37</v>
+        <v>329.03</v>
       </c>
       <c r="D140" t="s">
         <v>76</v>
@@ -5437,10 +5491,10 @@
         <v>19</v>
       </c>
       <c r="B141" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C141">
-        <v>357.91</v>
+        <v>434.37</v>
       </c>
       <c r="D141" t="s">
         <v>76</v>
@@ -5451,10 +5505,10 @@
         <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>45</v>
-      </c>
-      <c r="C142" t="s">
-        <v>76</v>
+        <v>33</v>
+      </c>
+      <c r="C142">
+        <v>357.91</v>
       </c>
       <c r="D142" t="s">
         <v>76</v>
@@ -5465,10 +5519,10 @@
         <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>60</v>
-      </c>
-      <c r="C143">
-        <v>473.66</v>
+        <v>45</v>
+      </c>
+      <c r="C143" t="s">
+        <v>76</v>
       </c>
       <c r="D143" t="s">
         <v>76</v>
@@ -5479,10 +5533,10 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C144">
-        <v>168.69</v>
+        <v>473.66</v>
       </c>
       <c r="D144" t="s">
         <v>76</v>
@@ -5493,27 +5547,27 @@
         <v>19</v>
       </c>
       <c r="B145" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C145">
-        <v>663.71</v>
-      </c>
-      <c r="D145">
-        <v>30.712</v>
+        <v>168.69</v>
+      </c>
+      <c r="D145" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C146">
-        <v>599.28</v>
-      </c>
-      <c r="D146" t="s">
-        <v>76</v>
+        <v>663.71</v>
+      </c>
+      <c r="D146">
+        <v>30.712</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,10 +5575,10 @@
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C147">
-        <v>459.22</v>
+        <v>599.28</v>
       </c>
       <c r="D147" t="s">
         <v>76</v>
@@ -5535,10 +5589,10 @@
         <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C148">
-        <v>314.02999999999997</v>
+        <v>459.22</v>
       </c>
       <c r="D148" t="s">
         <v>76</v>
@@ -5549,10 +5603,10 @@
         <v>20</v>
       </c>
       <c r="B149" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C149">
-        <v>436.14</v>
+        <v>314.02999999999997</v>
       </c>
       <c r="D149" t="s">
         <v>76</v>
@@ -5563,10 +5617,10 @@
         <v>20</v>
       </c>
       <c r="B150" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C150">
-        <v>138.38999999999999</v>
+        <v>436.14</v>
       </c>
       <c r="D150" t="s">
         <v>76</v>
@@ -5577,10 +5631,10 @@
         <v>20</v>
       </c>
       <c r="B151" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C151">
-        <v>599.28</v>
+        <v>138.38999999999999</v>
       </c>
       <c r="D151" t="s">
         <v>76</v>
@@ -5588,13 +5642,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C152">
-        <v>275.75</v>
+        <v>599.28</v>
       </c>
       <c r="D152" t="s">
         <v>76</v>
@@ -5605,10 +5659,10 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C153">
-        <v>288.2</v>
+        <v>275.75</v>
       </c>
       <c r="D153" t="s">
         <v>76</v>
@@ -5619,13 +5673,13 @@
         <v>21</v>
       </c>
       <c r="B154" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C154">
-        <v>387.25</v>
-      </c>
-      <c r="D154">
-        <v>94.462999999999994</v>
+        <v>288.2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5633,13 +5687,13 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C155">
-        <v>375.51</v>
-      </c>
-      <c r="D155" t="s">
-        <v>76</v>
+        <v>387.25</v>
+      </c>
+      <c r="D155">
+        <v>94.462999999999994</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5647,10 +5701,10 @@
         <v>21</v>
       </c>
       <c r="B156" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C156">
-        <v>449.83</v>
+        <v>375.51</v>
       </c>
       <c r="D156" t="s">
         <v>76</v>
@@ -5661,10 +5715,10 @@
         <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C157">
-        <v>203.76</v>
+        <v>449.83</v>
       </c>
       <c r="D157" t="s">
         <v>76</v>
@@ -5672,13 +5726,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B158" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C158">
-        <v>398.35</v>
+        <v>203.76</v>
       </c>
       <c r="D158" t="s">
         <v>76</v>
@@ -5689,10 +5743,10 @@
         <v>22</v>
       </c>
       <c r="B159" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C159">
-        <v>453.13</v>
+        <v>398.35</v>
       </c>
       <c r="D159" t="s">
         <v>76</v>
@@ -5703,10 +5757,10 @@
         <v>22</v>
       </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C160">
-        <v>437.75</v>
+        <v>453.13</v>
       </c>
       <c r="D160" t="s">
         <v>76</v>
@@ -5717,56 +5771,56 @@
         <v>22</v>
       </c>
       <c r="B161" t="s">
+        <v>25</v>
+      </c>
+      <c r="C161">
+        <v>437.75</v>
+      </c>
+      <c r="D161" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>22</v>
+      </c>
+      <c r="B162" t="s">
         <v>26</v>
       </c>
-      <c r="C161">
+      <c r="C162">
         <v>818.79</v>
       </c>
-      <c r="D161" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
+      <c r="D162" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C162" s="4">
+      <c r="C163" s="4">
         <v>818.79</v>
       </c>
-      <c r="D162" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E162" s="6"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>22</v>
-      </c>
-      <c r="B163" t="s">
-        <v>27</v>
-      </c>
-      <c r="C163">
-        <v>332.21</v>
-      </c>
-      <c r="D163">
-        <v>17.309000000000001</v>
-      </c>
+      <c r="D163" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E163" s="6"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>22</v>
       </c>
       <c r="B164" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C164">
-        <v>625.16999999999996</v>
-      </c>
-      <c r="D164" t="s">
-        <v>76</v>
+        <v>332.21</v>
+      </c>
+      <c r="D164">
+        <v>17.309000000000001</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5774,10 +5828,10 @@
         <v>22</v>
       </c>
       <c r="B165" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C165">
-        <v>414.91</v>
+        <v>625.16999999999996</v>
       </c>
       <c r="D165" t="s">
         <v>76</v>
@@ -5788,10 +5842,10 @@
         <v>22</v>
       </c>
       <c r="B166" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C166">
-        <v>540.83000000000004</v>
+        <v>414.91</v>
       </c>
       <c r="D166" t="s">
         <v>76</v>
@@ -5802,10 +5856,10 @@
         <v>22</v>
       </c>
       <c r="B167" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C167">
-        <v>1195.3</v>
+        <v>540.83000000000004</v>
       </c>
       <c r="D167" t="s">
         <v>76</v>
@@ -5816,10 +5870,10 @@
         <v>22</v>
       </c>
       <c r="B168" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C168">
-        <v>453.13</v>
+        <v>1195.3</v>
       </c>
       <c r="D168" t="s">
         <v>76</v>
@@ -5827,13 +5881,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B169" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C169">
-        <v>352.19</v>
+        <v>453.13</v>
       </c>
       <c r="D169" t="s">
         <v>76</v>
@@ -5844,41 +5898,41 @@
         <v>23</v>
       </c>
       <c r="B170" t="s">
+        <v>25</v>
+      </c>
+      <c r="C170">
+        <v>352.19</v>
+      </c>
+      <c r="D170" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>23</v>
+      </c>
+      <c r="B171" t="s">
         <v>26</v>
       </c>
-      <c r="C170">
+      <c r="C171">
         <v>498.6</v>
       </c>
-      <c r="D170" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="4" t="s">
+      <c r="D171" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C171" s="4">
+      <c r="C172" s="4">
         <v>498.6</v>
       </c>
-      <c r="D171" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>23</v>
-      </c>
-      <c r="B172" t="s">
-        <v>27</v>
-      </c>
-      <c r="C172">
-        <v>350.99</v>
-      </c>
-      <c r="D172">
-        <v>28</v>
+      <c r="D172" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -5886,13 +5940,13 @@
         <v>23</v>
       </c>
       <c r="B173" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C173">
-        <v>269.68</v>
-      </c>
-      <c r="D173" t="s">
-        <v>76</v>
+        <v>350.99</v>
+      </c>
+      <c r="D173">
+        <v>28</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5900,10 +5954,10 @@
         <v>23</v>
       </c>
       <c r="B174" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C174">
-        <v>376.57</v>
+        <v>269.68</v>
       </c>
       <c r="D174" t="s">
         <v>76</v>
@@ -5914,10 +5968,10 @@
         <v>23</v>
       </c>
       <c r="B175" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C175">
-        <v>554.5</v>
+        <v>376.57</v>
       </c>
       <c r="D175" t="s">
         <v>76</v>
@@ -5928,10 +5982,10 @@
         <v>23</v>
       </c>
       <c r="B176" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C176">
-        <v>332.15</v>
+        <v>554.5</v>
       </c>
       <c r="D176" t="s">
         <v>76</v>
@@ -5942,10 +5996,10 @@
         <v>23</v>
       </c>
       <c r="B177" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C177">
-        <v>549.42999999999995</v>
+        <v>332.15</v>
       </c>
       <c r="D177" t="s">
         <v>76</v>
@@ -5956,10 +6010,10 @@
         <v>23</v>
       </c>
       <c r="B178" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C178">
-        <v>650.24</v>
+        <v>549.42999999999995</v>
       </c>
       <c r="D178" t="s">
         <v>76</v>
@@ -5970,10 +6024,10 @@
         <v>23</v>
       </c>
       <c r="B179" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C179">
-        <v>605.45000000000005</v>
+        <v>650.24</v>
       </c>
       <c r="D179" t="s">
         <v>76</v>
@@ -5984,10 +6038,10 @@
         <v>23</v>
       </c>
       <c r="B180" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C180">
-        <v>536.66</v>
+        <v>605.45000000000005</v>
       </c>
       <c r="D180" t="s">
         <v>76</v>
@@ -5998,10 +6052,10 @@
         <v>23</v>
       </c>
       <c r="B181" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C181">
-        <v>846.19</v>
+        <v>536.66</v>
       </c>
       <c r="D181" t="s">
         <v>76</v>
@@ -6012,10 +6066,10 @@
         <v>23</v>
       </c>
       <c r="B182" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C182">
-        <v>321.70999999999998</v>
+        <v>846.19</v>
       </c>
       <c r="D182" t="s">
         <v>76</v>
@@ -6026,10 +6080,10 @@
         <v>23</v>
       </c>
       <c r="B183" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C183">
-        <v>486.88</v>
+        <v>321.70999999999998</v>
       </c>
       <c r="D183" t="s">
         <v>76</v>
@@ -6040,10 +6094,10 @@
         <v>23</v>
       </c>
       <c r="B184" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C184">
-        <v>750.06</v>
+        <v>486.88</v>
       </c>
       <c r="D184" t="s">
         <v>76</v>
@@ -6054,10 +6108,10 @@
         <v>23</v>
       </c>
       <c r="B185" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C185">
-        <v>389.9</v>
+        <v>750.06</v>
       </c>
       <c r="D185" t="s">
         <v>76</v>
@@ -6068,10 +6122,10 @@
         <v>23</v>
       </c>
       <c r="B186" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C186">
-        <v>564.85</v>
+        <v>389.9</v>
       </c>
       <c r="D186" t="s">
         <v>76</v>
@@ -6079,13 +6133,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B187" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C187">
-        <v>393.71</v>
+        <v>564.85</v>
       </c>
       <c r="D187" t="s">
         <v>76</v>
@@ -6096,10 +6150,10 @@
         <v>24</v>
       </c>
       <c r="B188" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C188">
-        <v>289.76</v>
+        <v>393.71</v>
       </c>
       <c r="D188" t="s">
         <v>76</v>
@@ -6110,10 +6164,10 @@
         <v>24</v>
       </c>
       <c r="B189" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C189">
-        <v>488.18</v>
+        <v>289.76</v>
       </c>
       <c r="D189" t="s">
         <v>76</v>
@@ -6124,10 +6178,10 @@
         <v>24</v>
       </c>
       <c r="B190" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C190">
-        <v>609.87</v>
+        <v>488.18</v>
       </c>
       <c r="D190" t="s">
         <v>76</v>
@@ -6138,10 +6192,10 @@
         <v>24</v>
       </c>
       <c r="B191" t="s">
-        <v>45</v>
-      </c>
-      <c r="C191" t="s">
-        <v>76</v>
+        <v>39</v>
+      </c>
+      <c r="C191">
+        <v>609.87</v>
       </c>
       <c r="D191" t="s">
         <v>76</v>
@@ -6152,7 +6206,7 @@
         <v>24</v>
       </c>
       <c r="B192" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C192" t="s">
         <v>76</v>
@@ -6166,54 +6220,54 @@
         <v>24</v>
       </c>
       <c r="B193" t="s">
-        <v>60</v>
-      </c>
-      <c r="C193">
-        <v>405.78</v>
-      </c>
-      <c r="D193">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C193" t="s">
+        <v>76</v>
+      </c>
+      <c r="D193" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>24</v>
+      </c>
+      <c r="B194" t="s">
+        <v>60</v>
+      </c>
+      <c r="C194">
+        <v>405.78</v>
+      </c>
+      <c r="D194">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>25</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B195" t="s">
         <v>26</v>
       </c>
-      <c r="C194">
+      <c r="C195">
         <v>547.44000000000005</v>
       </c>
-      <c r="D194" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="4" t="s">
+      <c r="D195" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B196" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C195" s="4">
+      <c r="C196" s="4">
         <v>547.44000000000005</v>
       </c>
-      <c r="D195" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>25</v>
-      </c>
-      <c r="B196" t="s">
-        <v>27</v>
-      </c>
-      <c r="C196">
-        <v>287.26</v>
-      </c>
-      <c r="D196" t="s">
+      <c r="D196" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6222,10 +6276,10 @@
         <v>25</v>
       </c>
       <c r="B197" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C197">
-        <v>340.81</v>
+        <v>287.26</v>
       </c>
       <c r="D197" t="s">
         <v>76</v>
@@ -6236,10 +6290,10 @@
         <v>25</v>
       </c>
       <c r="B198" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C198">
-        <v>338.47</v>
+        <v>340.81</v>
       </c>
       <c r="D198" t="s">
         <v>76</v>
@@ -6250,10 +6304,10 @@
         <v>25</v>
       </c>
       <c r="B199" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C199">
-        <v>340.81</v>
+        <v>338.47</v>
       </c>
       <c r="D199" t="s">
         <v>76</v>
@@ -6264,10 +6318,10 @@
         <v>25</v>
       </c>
       <c r="B200" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C200">
-        <v>516.30999999999995</v>
+        <v>340.81</v>
       </c>
       <c r="D200" t="s">
         <v>76</v>
@@ -6278,10 +6332,10 @@
         <v>25</v>
       </c>
       <c r="B201" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C201">
-        <v>389.74</v>
+        <v>516.30999999999995</v>
       </c>
       <c r="D201" t="s">
         <v>76</v>
@@ -6292,10 +6346,10 @@
         <v>25</v>
       </c>
       <c r="B202" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C202">
-        <v>316.60000000000002</v>
+        <v>389.74</v>
       </c>
       <c r="D202" t="s">
         <v>76</v>
@@ -6306,27 +6360,27 @@
         <v>25</v>
       </c>
       <c r="B203" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C203">
-        <v>261.23</v>
-      </c>
-      <c r="D203">
-        <v>8</v>
+        <v>316.60000000000002</v>
+      </c>
+      <c r="D203" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B204" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C204">
-        <v>396.81</v>
+        <v>261.23</v>
       </c>
       <c r="D204">
-        <v>15.14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -6334,13 +6388,13 @@
         <v>26</v>
       </c>
       <c r="B205" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C205">
-        <v>490.95</v>
-      </c>
-      <c r="D205" t="s">
-        <v>76</v>
+        <v>396.81</v>
+      </c>
+      <c r="D205">
+        <v>15.14</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -6348,10 +6402,10 @@
         <v>26</v>
       </c>
       <c r="B206" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C206">
-        <v>868.11</v>
+        <v>490.95</v>
       </c>
       <c r="D206" t="s">
         <v>76</v>
@@ -6362,10 +6416,10 @@
         <v>26</v>
       </c>
       <c r="B207" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="C207">
-        <v>331.78</v>
+        <v>868.11</v>
       </c>
       <c r="D207" t="s">
         <v>76</v>
@@ -6376,27 +6430,27 @@
         <v>26</v>
       </c>
       <c r="B208" t="s">
+        <v>67</v>
+      </c>
+      <c r="C208">
+        <v>331.78</v>
+      </c>
+      <c r="D208" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>26</v>
+      </c>
+      <c r="B209" t="s">
         <v>68</v>
       </c>
-      <c r="C208">
+      <c r="C209">
         <v>809.96</v>
       </c>
-      <c r="D208" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C209" s="4">
-        <v>396.81</v>
-      </c>
-      <c r="D209" s="4">
-        <v>15.14</v>
+      <c r="D209" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -6404,13 +6458,13 @@
         <v>91</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C210" s="4">
-        <v>490.95</v>
-      </c>
-      <c r="D210" s="4" t="s">
-        <v>76</v>
+        <v>396.81</v>
+      </c>
+      <c r="D210" s="4">
+        <v>15.14</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -6418,10 +6472,10 @@
         <v>91</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C211" s="4">
-        <v>868.11</v>
+        <v>490.95</v>
       </c>
       <c r="D211" s="4" t="s">
         <v>76</v>
@@ -6432,10 +6486,10 @@
         <v>91</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="C212" s="4">
-        <v>331.78</v>
+        <v>868.11</v>
       </c>
       <c r="D212" s="4" t="s">
         <v>76</v>
@@ -6446,26 +6500,26 @@
         <v>91</v>
       </c>
       <c r="B213" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C213" s="4">
+        <v>331.78</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B214" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C213" s="4">
+      <c r="C214" s="4">
         <v>809.96</v>
       </c>
-      <c r="D213" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>27</v>
-      </c>
-      <c r="B214" t="s">
-        <v>28</v>
-      </c>
-      <c r="C214">
-        <v>278.45</v>
-      </c>
-      <c r="D214" t="s">
+      <c r="D214" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6474,10 +6528,10 @@
         <v>27</v>
       </c>
       <c r="B215" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C215">
-        <v>175.41</v>
+        <v>278.45</v>
       </c>
       <c r="D215" t="s">
         <v>76</v>
@@ -6488,10 +6542,10 @@
         <v>27</v>
       </c>
       <c r="B216" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C216">
-        <v>226.38</v>
+        <v>175.41</v>
       </c>
       <c r="D216" t="s">
         <v>76</v>
@@ -6502,10 +6556,10 @@
         <v>27</v>
       </c>
       <c r="B217" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C217">
-        <v>375.92</v>
+        <v>226.38</v>
       </c>
       <c r="D217" t="s">
         <v>76</v>
@@ -6516,10 +6570,10 @@
         <v>27</v>
       </c>
       <c r="B218" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C218">
-        <v>353.37</v>
+        <v>375.92</v>
       </c>
       <c r="D218" t="s">
         <v>76</v>
@@ -6530,10 +6584,10 @@
         <v>27</v>
       </c>
       <c r="B219" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C219">
-        <v>479.16</v>
+        <v>353.37</v>
       </c>
       <c r="D219" t="s">
         <v>76</v>
@@ -6544,10 +6598,10 @@
         <v>27</v>
       </c>
       <c r="B220" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C220">
-        <v>358.55</v>
+        <v>479.16</v>
       </c>
       <c r="D220" t="s">
         <v>76</v>
@@ -6558,13 +6612,13 @@
         <v>27</v>
       </c>
       <c r="B221" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C221">
-        <v>646.1</v>
-      </c>
-      <c r="D221">
-        <v>13.195</v>
+        <v>358.55</v>
+      </c>
+      <c r="D221" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -6572,13 +6626,13 @@
         <v>27</v>
       </c>
       <c r="B222" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C222">
-        <v>1481.3</v>
+        <v>646.1</v>
       </c>
       <c r="D222">
-        <v>21.216999999999999</v>
+        <v>13.195</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -6586,13 +6640,13 @@
         <v>27</v>
       </c>
       <c r="B223" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C223">
-        <v>523.83000000000004</v>
+        <v>1481.3</v>
       </c>
       <c r="D223">
-        <v>8.4243000000000006</v>
+        <v>21.216999999999999</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6600,13 +6654,13 @@
         <v>27</v>
       </c>
       <c r="B224" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C224">
-        <v>2990</v>
+        <v>523.83000000000004</v>
       </c>
       <c r="D224">
-        <v>66.108999999999995</v>
+        <v>8.4243000000000006</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -6614,13 +6668,13 @@
         <v>27</v>
       </c>
       <c r="B225" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C225">
-        <v>310.91000000000003</v>
+        <v>2990</v>
       </c>
       <c r="D225">
-        <v>8</v>
+        <v>66.108999999999995</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -6628,13 +6682,13 @@
         <v>27</v>
       </c>
       <c r="B226" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C226">
-        <v>360.7</v>
-      </c>
-      <c r="D226" t="s">
-        <v>76</v>
+        <v>310.91000000000003</v>
+      </c>
+      <c r="D226">
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -6642,13 +6696,13 @@
         <v>27</v>
       </c>
       <c r="B227" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C227">
-        <v>238.77</v>
-      </c>
-      <c r="D227">
-        <v>8</v>
+        <v>360.7</v>
+      </c>
+      <c r="D227" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -6656,13 +6710,13 @@
         <v>27</v>
       </c>
       <c r="B228" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C228">
-        <v>377.16</v>
+        <v>238.77</v>
       </c>
       <c r="D228">
-        <v>22.265000000000001</v>
+        <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -6670,13 +6724,13 @@
         <v>27</v>
       </c>
       <c r="B229" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C229">
-        <v>855.01</v>
+        <v>377.16</v>
       </c>
       <c r="D229">
-        <v>32.131999999999998</v>
+        <v>22.265000000000001</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -6684,13 +6738,13 @@
         <v>27</v>
       </c>
       <c r="B230" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C230">
-        <v>1067.9000000000001</v>
+        <v>855.01</v>
       </c>
       <c r="D230">
-        <v>8.0009999999999994</v>
+        <v>32.131999999999998</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -6698,13 +6752,13 @@
         <v>27</v>
       </c>
       <c r="B231" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C231">
-        <v>391.04</v>
-      </c>
-      <c r="D231" t="s">
-        <v>76</v>
+        <v>1067.9000000000001</v>
+      </c>
+      <c r="D231">
+        <v>8.0009999999999994</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -6712,10 +6766,10 @@
         <v>27</v>
       </c>
       <c r="B232" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C232">
-        <v>1023.1</v>
+        <v>391.04</v>
       </c>
       <c r="D232" t="s">
         <v>76</v>
@@ -6726,10 +6780,10 @@
         <v>27</v>
       </c>
       <c r="B233" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C233">
-        <v>539.67999999999995</v>
+        <v>1023.1</v>
       </c>
       <c r="D233" t="s">
         <v>76</v>
@@ -6740,10 +6794,10 @@
         <v>27</v>
       </c>
       <c r="B234" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C234">
-        <v>376.25</v>
+        <v>539.67999999999995</v>
       </c>
       <c r="D234" t="s">
         <v>76</v>
@@ -6754,10 +6808,10 @@
         <v>27</v>
       </c>
       <c r="B235" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C235">
-        <v>354.23</v>
+        <v>376.25</v>
       </c>
       <c r="D235" t="s">
         <v>76</v>
@@ -6768,10 +6822,10 @@
         <v>27</v>
       </c>
       <c r="B236" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C236">
-        <v>2235.1</v>
+        <v>354.23</v>
       </c>
       <c r="D236" t="s">
         <v>76</v>
@@ -6782,10 +6836,10 @@
         <v>27</v>
       </c>
       <c r="B237" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C237">
-        <v>1460.8</v>
+        <v>2235.1</v>
       </c>
       <c r="D237" t="s">
         <v>76</v>
@@ -6796,10 +6850,10 @@
         <v>27</v>
       </c>
       <c r="B238" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C238">
-        <v>1047</v>
+        <v>1460.8</v>
       </c>
       <c r="D238" t="s">
         <v>76</v>
@@ -6810,10 +6864,10 @@
         <v>27</v>
       </c>
       <c r="B239" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C239">
-        <v>840.44</v>
+        <v>1047</v>
       </c>
       <c r="D239" t="s">
         <v>76</v>
@@ -6824,13 +6878,13 @@
         <v>27</v>
       </c>
       <c r="B240" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C240">
-        <v>1481.3</v>
-      </c>
-      <c r="D240">
-        <v>21.216999999999999</v>
+        <v>840.44</v>
+      </c>
+      <c r="D240" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -6838,13 +6892,13 @@
         <v>27</v>
       </c>
       <c r="B241" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C241">
-        <v>134.41</v>
-      </c>
-      <c r="D241" t="s">
-        <v>76</v>
+        <v>1481.3</v>
+      </c>
+      <c r="D241">
+        <v>21.216999999999999</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -6852,10 +6906,10 @@
         <v>27</v>
       </c>
       <c r="B242" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C242">
-        <v>30.571000000000002</v>
+        <v>134.41</v>
       </c>
       <c r="D242" t="s">
         <v>76</v>
@@ -6866,10 +6920,10 @@
         <v>27</v>
       </c>
       <c r="B243" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C243">
-        <v>95.406000000000006</v>
+        <v>30.571000000000002</v>
       </c>
       <c r="D243" t="s">
         <v>76</v>
@@ -6880,10 +6934,10 @@
         <v>27</v>
       </c>
       <c r="B244" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C244">
-        <v>112.01</v>
+        <v>95.406000000000006</v>
       </c>
       <c r="D244" t="s">
         <v>76</v>
@@ -6894,10 +6948,10 @@
         <v>27</v>
       </c>
       <c r="B245" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C245">
-        <v>142.66</v>
+        <v>112.01</v>
       </c>
       <c r="D245" t="s">
         <v>76</v>
@@ -6908,10 +6962,10 @@
         <v>27</v>
       </c>
       <c r="B246" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C246">
-        <v>171.61</v>
+        <v>142.66</v>
       </c>
       <c r="D246" t="s">
         <v>76</v>
@@ -6922,10 +6976,10 @@
         <v>27</v>
       </c>
       <c r="B247" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C247">
-        <v>142.57</v>
+        <v>171.61</v>
       </c>
       <c r="D247" t="s">
         <v>76</v>
@@ -6936,10 +6990,10 @@
         <v>27</v>
       </c>
       <c r="B248" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C248">
-        <v>128.03</v>
+        <v>142.57</v>
       </c>
       <c r="D248" t="s">
         <v>76</v>
@@ -6950,10 +7004,10 @@
         <v>27</v>
       </c>
       <c r="B249" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C249">
-        <v>270</v>
+        <v>128.03</v>
       </c>
       <c r="D249" t="s">
         <v>76</v>
@@ -6964,10 +7018,10 @@
         <v>27</v>
       </c>
       <c r="B250" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C250">
-        <v>161.55000000000001</v>
+        <v>270</v>
       </c>
       <c r="D250" t="s">
         <v>76</v>
@@ -6978,10 +7032,10 @@
         <v>27</v>
       </c>
       <c r="B251" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C251">
-        <v>317.43</v>
+        <v>161.55000000000001</v>
       </c>
       <c r="D251" t="s">
         <v>76</v>
@@ -6992,27 +7046,27 @@
         <v>27</v>
       </c>
       <c r="B252" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C252">
-        <v>228.58</v>
-      </c>
-      <c r="D252">
-        <v>9.5614000000000008</v>
+        <v>317.43</v>
+      </c>
+      <c r="D252" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B253" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C253">
-        <v>233.21</v>
-      </c>
-      <c r="D253" t="s">
-        <v>76</v>
+        <v>228.58</v>
+      </c>
+      <c r="D253">
+        <v>9.5614000000000008</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -7020,13 +7074,13 @@
         <v>28</v>
       </c>
       <c r="B254" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C254">
-        <v>157.83000000000001</v>
-      </c>
-      <c r="D254">
-        <v>8.3461999999999996</v>
+        <v>233.21</v>
+      </c>
+      <c r="D254" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,13 +7088,13 @@
         <v>28</v>
       </c>
       <c r="B255" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C255">
-        <v>290.16000000000003</v>
+        <v>157.83000000000001</v>
       </c>
       <c r="D255">
-        <v>8</v>
+        <v>8.3461999999999996</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -7048,27 +7102,27 @@
         <v>28</v>
       </c>
       <c r="B256" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C256">
-        <v>398.1</v>
-      </c>
-      <c r="D256" t="s">
-        <v>76</v>
+        <v>290.16000000000003</v>
+      </c>
+      <c r="D256">
+        <v>8</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B257" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C257">
-        <v>144.72</v>
-      </c>
-      <c r="D257">
-        <v>11.95</v>
+        <v>398.1</v>
+      </c>
+      <c r="D257" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -7076,13 +7130,13 @@
         <v>29</v>
       </c>
       <c r="B258" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C258">
-        <v>210.13</v>
-      </c>
-      <c r="D258" t="s">
-        <v>76</v>
+        <v>144.72</v>
+      </c>
+      <c r="D258">
+        <v>11.95</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -7090,10 +7144,10 @@
         <v>29</v>
       </c>
       <c r="B259" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C259">
-        <v>182.18</v>
+        <v>210.13</v>
       </c>
       <c r="D259" t="s">
         <v>76</v>
@@ -7101,16 +7155,16 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B260" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C260">
-        <v>200.62</v>
-      </c>
-      <c r="D260">
-        <v>49.975000000000001</v>
+        <v>182.18</v>
+      </c>
+      <c r="D260" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -7118,13 +7172,13 @@
         <v>30</v>
       </c>
       <c r="B261" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C261">
-        <v>100.01</v>
+        <v>200.62</v>
       </c>
       <c r="D261">
-        <v>49.529000000000003</v>
+        <v>49.975000000000001</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -7132,13 +7186,13 @@
         <v>30</v>
       </c>
       <c r="B262" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C262">
-        <v>100.58</v>
+        <v>100.01</v>
       </c>
       <c r="D262">
-        <v>49.999000000000002</v>
+        <v>49.529000000000003</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -7146,13 +7200,13 @@
         <v>30</v>
       </c>
       <c r="B263" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C263">
-        <v>80.100999999999999</v>
+        <v>100.58</v>
       </c>
       <c r="D263">
-        <v>39.706000000000003</v>
+        <v>49.999000000000002</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -7160,13 +7214,13 @@
         <v>30</v>
       </c>
       <c r="B264" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C264">
-        <v>90.102000000000004</v>
+        <v>80.100999999999999</v>
       </c>
       <c r="D264">
-        <v>35.343000000000004</v>
+        <v>39.706000000000003</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -7174,13 +7228,13 @@
         <v>30</v>
       </c>
       <c r="B265" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C265">
-        <v>294.99</v>
-      </c>
-      <c r="D265" t="s">
-        <v>76</v>
+        <v>90.102000000000004</v>
+      </c>
+      <c r="D265">
+        <v>35.343000000000004</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -7188,13 +7242,13 @@
         <v>30</v>
       </c>
       <c r="B266" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C266">
-        <v>100.53</v>
-      </c>
-      <c r="D266">
-        <v>31.234000000000002</v>
+        <v>294.99</v>
+      </c>
+      <c r="D266" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -7202,13 +7256,13 @@
         <v>30</v>
       </c>
       <c r="B267" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C267">
-        <v>189.86</v>
-      </c>
-      <c r="D267" t="s">
-        <v>76</v>
+        <v>100.53</v>
+      </c>
+      <c r="D267">
+        <v>31.234000000000002</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -7216,10 +7270,10 @@
         <v>30</v>
       </c>
       <c r="B268" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C268">
-        <v>371.59</v>
+        <v>189.86</v>
       </c>
       <c r="D268" t="s">
         <v>76</v>
@@ -7230,10 +7284,10 @@
         <v>30</v>
       </c>
       <c r="B269" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C269">
-        <v>327.31</v>
+        <v>371.59</v>
       </c>
       <c r="D269" t="s">
         <v>76</v>
@@ -7244,267 +7298,267 @@
         <v>30</v>
       </c>
       <c r="B270" t="s">
+        <v>70</v>
+      </c>
+      <c r="C270">
+        <v>327.31</v>
+      </c>
+      <c r="D270" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>30</v>
+      </c>
+      <c r="B271" t="s">
         <v>71</v>
       </c>
-      <c r="C270">
+      <c r="C271">
         <v>283.77999999999997</v>
       </c>
-      <c r="D270" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B271" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C271" s="2">
-        <v>630.28474750541602</v>
-      </c>
-      <c r="D271" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E271" s="6"/>
+      <c r="D271" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B272" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C272" s="2">
+        <v>628.98238399086097</v>
+      </c>
+      <c r="D272" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E272" s="6"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B273" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C272" s="2">
-        <v>189.27611672354701</v>
-      </c>
-      <c r="D272" s="2">
+      <c r="C273" s="2">
+        <v>189.27590000000001</v>
+      </c>
+      <c r="D273" s="2">
         <v>8</v>
       </c>
-      <c r="E272" s="6"/>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>31</v>
-      </c>
-      <c r="B273" t="s">
-        <v>34</v>
-      </c>
-      <c r="C273">
-        <v>241.94</v>
-      </c>
-      <c r="D273" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E273" s="6"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>31</v>
       </c>
       <c r="B274" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C274">
-        <v>188.61</v>
+        <v>241.94</v>
       </c>
       <c r="D274" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>31</v>
       </c>
       <c r="B275" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C275">
-        <v>260.99</v>
+        <v>188.61</v>
       </c>
       <c r="D275" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>31</v>
       </c>
       <c r="B276" t="s">
+        <v>36</v>
+      </c>
+      <c r="C276">
+        <v>260.99</v>
+      </c>
+      <c r="D276" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>31</v>
+      </c>
+      <c r="B277" t="s">
         <v>39</v>
       </c>
-      <c r="C276">
+      <c r="C277">
         <v>784.51</v>
       </c>
-      <c r="D276" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>32</v>
-      </c>
-      <c r="B277" t="s">
-        <v>33</v>
-      </c>
-      <c r="C277">
-        <v>389.23</v>
-      </c>
       <c r="D277" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>32</v>
       </c>
       <c r="B278" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C278">
-        <v>528.21</v>
-      </c>
-      <c r="D278">
-        <v>52.305</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+        <v>389.23</v>
+      </c>
+      <c r="D278" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>32</v>
       </c>
       <c r="B279" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C279">
-        <v>313.25</v>
-      </c>
-      <c r="D279" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+        <v>528.21</v>
+      </c>
+      <c r="D279">
+        <v>52.305</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>32</v>
       </c>
       <c r="B280" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C280">
-        <v>440.99</v>
+        <v>313.25</v>
       </c>
       <c r="D280" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>32</v>
       </c>
       <c r="B281" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C281">
-        <v>799.66</v>
+        <v>440.99</v>
       </c>
       <c r="D281" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>32</v>
       </c>
       <c r="B282" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C282">
-        <v>486.62</v>
+        <v>799.66</v>
       </c>
       <c r="D282" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>32</v>
       </c>
       <c r="B283" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C283">
-        <v>307.89</v>
-      </c>
-      <c r="D283">
-        <v>41.331000000000003</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+        <v>486.62</v>
+      </c>
+      <c r="D283" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>32</v>
       </c>
       <c r="B284" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C284">
-        <v>440.99</v>
-      </c>
-      <c r="D284" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307.89</v>
+      </c>
+      <c r="D284">
+        <v>41.331000000000003</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>32</v>
       </c>
       <c r="B285" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C285">
-        <v>656.8</v>
+        <v>440.99</v>
       </c>
       <c r="D285" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>32</v>
       </c>
       <c r="B286" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C286">
-        <v>172.57</v>
-      </c>
-      <c r="D286">
-        <v>9.2665000000000006</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+        <v>656.8</v>
+      </c>
+      <c r="D286" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>32</v>
       </c>
       <c r="B287" t="s">
+        <v>67</v>
+      </c>
+      <c r="C287">
+        <v>172.57</v>
+      </c>
+      <c r="D287">
+        <v>9.2665000000000006</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>32</v>
+      </c>
+      <c r="B288" t="s">
         <v>68</v>
       </c>
-      <c r="C287">
+      <c r="C288">
         <v>485.03</v>
       </c>
-      <c r="D287">
+      <c r="D288">
         <v>8.0012000000000008</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>33</v>
-      </c>
-      <c r="B288" t="s">
-        <v>39</v>
-      </c>
-      <c r="C288">
-        <v>245.07</v>
-      </c>
-      <c r="D288" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -7512,10 +7566,10 @@
         <v>33</v>
       </c>
       <c r="B289" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C289">
-        <v>762.86</v>
+        <v>245.07</v>
       </c>
       <c r="D289" t="s">
         <v>76</v>
@@ -7526,13 +7580,13 @@
         <v>33</v>
       </c>
       <c r="B290" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C290">
-        <v>81.542000000000002</v>
-      </c>
-      <c r="D290">
-        <v>79.266000000000005</v>
+        <v>762.86</v>
+      </c>
+      <c r="D290" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -7540,27 +7594,27 @@
         <v>33</v>
       </c>
       <c r="B291" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C291">
-        <v>451.48</v>
+        <v>81.542000000000002</v>
       </c>
       <c r="D291">
-        <v>8.1809999999999992</v>
+        <v>79.266000000000005</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B292" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C292">
-        <v>381.98</v>
-      </c>
-      <c r="D292" t="s">
-        <v>76</v>
+        <v>451.48</v>
+      </c>
+      <c r="D292">
+        <v>8.1809999999999992</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -7568,10 +7622,10 @@
         <v>34</v>
       </c>
       <c r="B293" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C293">
-        <v>101.61</v>
+        <v>381.98</v>
       </c>
       <c r="D293" t="s">
         <v>76</v>
@@ -7579,13 +7633,13 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B294" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C294">
-        <v>812.26</v>
+        <v>101.61</v>
       </c>
       <c r="D294" t="s">
         <v>76</v>
@@ -7593,13 +7647,13 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B295" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C295">
-        <v>609.87</v>
+        <v>812.26</v>
       </c>
       <c r="D295" t="s">
         <v>76</v>
@@ -7607,13 +7661,13 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B296" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C296">
-        <v>455.68</v>
+        <v>609.87</v>
       </c>
       <c r="D296" t="s">
         <v>76</v>
@@ -7624,10 +7678,10 @@
         <v>40</v>
       </c>
       <c r="B297" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C297">
-        <v>941.03</v>
+        <v>455.68</v>
       </c>
       <c r="D297" t="s">
         <v>76</v>
@@ -7638,38 +7692,38 @@
         <v>40</v>
       </c>
       <c r="B298" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C298">
-        <v>552.62</v>
-      </c>
-      <c r="D298">
-        <v>36.429000000000002</v>
+        <v>941.03</v>
+      </c>
+      <c r="D298" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B299" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C299">
-        <v>246.61</v>
-      </c>
-      <c r="D299" t="s">
-        <v>76</v>
+        <v>552.62</v>
+      </c>
+      <c r="D299">
+        <v>36.429000000000002</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B300" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C300">
-        <v>37.478999999999999</v>
+        <v>246.61</v>
       </c>
       <c r="D300" t="s">
         <v>76</v>
@@ -7680,10 +7734,10 @@
         <v>45</v>
       </c>
       <c r="B301" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C301">
-        <v>66.42</v>
+        <v>37.478999999999999</v>
       </c>
       <c r="D301" t="s">
         <v>76</v>
@@ -7694,10 +7748,10 @@
         <v>45</v>
       </c>
       <c r="B302" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C302">
-        <v>51.094999999999999</v>
+        <v>66.42</v>
       </c>
       <c r="D302" t="s">
         <v>76</v>
@@ -7708,10 +7762,10 @@
         <v>45</v>
       </c>
       <c r="B303" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C303">
-        <v>70.545000000000002</v>
+        <v>51.094999999999999</v>
       </c>
       <c r="D303" t="s">
         <v>76</v>
@@ -7722,10 +7776,10 @@
         <v>45</v>
       </c>
       <c r="B304" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C304">
-        <v>65.8</v>
+        <v>70.545000000000002</v>
       </c>
       <c r="D304" t="s">
         <v>76</v>
@@ -7736,10 +7790,10 @@
         <v>45</v>
       </c>
       <c r="B305" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C305">
-        <v>59.652000000000001</v>
+        <v>65.8</v>
       </c>
       <c r="D305" t="s">
         <v>76</v>
@@ -7750,10 +7804,10 @@
         <v>45</v>
       </c>
       <c r="B306" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C306">
-        <v>28.111000000000001</v>
+        <v>59.652000000000001</v>
       </c>
       <c r="D306" t="s">
         <v>76</v>
@@ -7764,10 +7818,10 @@
         <v>45</v>
       </c>
       <c r="B307" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C307">
-        <v>60.475999999999999</v>
+        <v>28.111000000000001</v>
       </c>
       <c r="D307" t="s">
         <v>76</v>
@@ -7778,10 +7832,10 @@
         <v>45</v>
       </c>
       <c r="B308" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C308">
-        <v>53.609000000000002</v>
+        <v>60.475999999999999</v>
       </c>
       <c r="D308" t="s">
         <v>76</v>
@@ -7792,10 +7846,10 @@
         <v>45</v>
       </c>
       <c r="B309" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C309">
-        <v>181.61</v>
+        <v>53.609000000000002</v>
       </c>
       <c r="D309" t="s">
         <v>76</v>
@@ -7806,10 +7860,10 @@
         <v>45</v>
       </c>
       <c r="B310" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C310">
-        <v>61.781999999999996</v>
+        <v>181.61</v>
       </c>
       <c r="D310" t="s">
         <v>76</v>
@@ -7820,10 +7874,10 @@
         <v>45</v>
       </c>
       <c r="B311" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C311">
-        <v>130.28</v>
+        <v>61.781999999999996</v>
       </c>
       <c r="D311" t="s">
         <v>76</v>
@@ -7831,13 +7885,13 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B312" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C312">
-        <v>9.1460000000000008</v>
+        <v>130.28</v>
       </c>
       <c r="D312" t="s">
         <v>76</v>
@@ -7848,10 +7902,10 @@
         <v>46</v>
       </c>
       <c r="B313" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C313">
-        <v>7.6875</v>
+        <v>9.1460000000000008</v>
       </c>
       <c r="D313" t="s">
         <v>76</v>
@@ -7862,10 +7916,10 @@
         <v>46</v>
       </c>
       <c r="B314" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C314">
-        <v>8.2898999999999994</v>
+        <v>7.6875</v>
       </c>
       <c r="D314" t="s">
         <v>76</v>
@@ -7876,10 +7930,10 @@
         <v>46</v>
       </c>
       <c r="B315" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C315">
-        <v>7.1798000000000002</v>
+        <v>8.2898999999999994</v>
       </c>
       <c r="D315" t="s">
         <v>76</v>
@@ -7890,10 +7944,10 @@
         <v>46</v>
       </c>
       <c r="B316" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C316">
-        <v>5.8745000000000003</v>
+        <v>7.1798000000000002</v>
       </c>
       <c r="D316" t="s">
         <v>76</v>
@@ -7901,13 +7955,13 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B317" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C317">
-        <v>27.890999999999998</v>
+        <v>5.8745000000000003</v>
       </c>
       <c r="D317" t="s">
         <v>76</v>
@@ -7918,10 +7972,10 @@
         <v>47</v>
       </c>
       <c r="B318" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C318">
-        <v>22.89</v>
+        <v>27.890999999999998</v>
       </c>
       <c r="D318" t="s">
         <v>76</v>
@@ -7932,10 +7986,10 @@
         <v>47</v>
       </c>
       <c r="B319" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C319">
-        <v>27.937000000000001</v>
+        <v>22.89</v>
       </c>
       <c r="D319" t="s">
         <v>76</v>
@@ -7946,10 +8000,10 @@
         <v>47</v>
       </c>
       <c r="B320" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C320">
-        <v>24.988</v>
+        <v>27.937000000000001</v>
       </c>
       <c r="D320" t="s">
         <v>76</v>
@@ -7960,10 +8014,10 @@
         <v>47</v>
       </c>
       <c r="B321" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C321">
-        <v>21.381</v>
+        <v>24.988</v>
       </c>
       <c r="D321" t="s">
         <v>76</v>
@@ -7974,10 +8028,10 @@
         <v>47</v>
       </c>
       <c r="B322" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C322">
-        <v>9.9114000000000004</v>
+        <v>21.381</v>
       </c>
       <c r="D322" t="s">
         <v>76</v>
@@ -7985,13 +8039,13 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B323" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C323">
-        <v>54.72</v>
+        <v>9.9114000000000004</v>
       </c>
       <c r="D323" t="s">
         <v>76</v>
@@ -8002,10 +8056,10 @@
         <v>48</v>
       </c>
       <c r="B324" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C324">
-        <v>43.679000000000002</v>
+        <v>54.72</v>
       </c>
       <c r="D324" t="s">
         <v>76</v>
@@ -8016,10 +8070,10 @@
         <v>48</v>
       </c>
       <c r="B325" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C325">
-        <v>61.006999999999998</v>
+        <v>43.679000000000002</v>
       </c>
       <c r="D325" t="s">
         <v>76</v>
@@ -8030,10 +8084,10 @@
         <v>48</v>
       </c>
       <c r="B326" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C326">
-        <v>56.588999999999999</v>
+        <v>61.006999999999998</v>
       </c>
       <c r="D326" t="s">
         <v>76</v>
@@ -8044,10 +8098,10 @@
         <v>48</v>
       </c>
       <c r="B327" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C327">
-        <v>50.96</v>
+        <v>56.588999999999999</v>
       </c>
       <c r="D327" t="s">
         <v>76</v>
@@ -8058,10 +8112,10 @@
         <v>48</v>
       </c>
       <c r="B328" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C328">
-        <v>24.044</v>
+        <v>50.96</v>
       </c>
       <c r="D328" t="s">
         <v>76</v>
@@ -8069,13 +8123,13 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B329" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C329">
-        <v>67.927000000000007</v>
+        <v>24.044</v>
       </c>
       <c r="D329" t="s">
         <v>76</v>
@@ -8086,10 +8140,10 @@
         <v>49</v>
       </c>
       <c r="B330" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C330">
-        <v>53.631</v>
+        <v>67.927000000000007</v>
       </c>
       <c r="D330" t="s">
         <v>76</v>
@@ -8100,10 +8154,10 @@
         <v>49</v>
       </c>
       <c r="B331" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C331">
-        <v>78.25</v>
+        <v>53.631</v>
       </c>
       <c r="D331" t="s">
         <v>76</v>
@@ -8114,10 +8168,10 @@
         <v>49</v>
       </c>
       <c r="B332" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C332">
-        <v>73.484999999999999</v>
+        <v>78.25</v>
       </c>
       <c r="D332" t="s">
         <v>76</v>
@@ -8128,10 +8182,10 @@
         <v>49</v>
       </c>
       <c r="B333" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C333">
-        <v>67.338999999999999</v>
+        <v>73.484999999999999</v>
       </c>
       <c r="D333" t="s">
         <v>76</v>
@@ -8139,13 +8193,13 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B334" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C334">
-        <v>33.261000000000003</v>
+        <v>67.338999999999999</v>
       </c>
       <c r="D334" t="s">
         <v>76</v>
@@ -8156,10 +8210,10 @@
         <v>50</v>
       </c>
       <c r="B335" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C335">
-        <v>28.048999999999999</v>
+        <v>33.261000000000003</v>
       </c>
       <c r="D335" t="s">
         <v>76</v>
@@ -8170,10 +8224,10 @@
         <v>50</v>
       </c>
       <c r="B336" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C336">
-        <v>29.599</v>
+        <v>28.048999999999999</v>
       </c>
       <c r="D336" t="s">
         <v>76</v>
@@ -8184,10 +8238,10 @@
         <v>50</v>
       </c>
       <c r="B337" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C337">
-        <v>25.497</v>
+        <v>29.599</v>
       </c>
       <c r="D337" t="s">
         <v>76</v>
@@ -8198,10 +8252,10 @@
         <v>50</v>
       </c>
       <c r="B338" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C338">
-        <v>20.706</v>
+        <v>25.497</v>
       </c>
       <c r="D338" t="s">
         <v>76</v>
@@ -8209,13 +8263,13 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B339" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C339">
-        <v>77.225999999999999</v>
+        <v>20.706</v>
       </c>
       <c r="D339" t="s">
         <v>76</v>
@@ -8226,10 +8280,10 @@
         <v>51</v>
       </c>
       <c r="B340" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C340">
-        <v>63.569000000000003</v>
+        <v>77.225999999999999</v>
       </c>
       <c r="D340" t="s">
         <v>76</v>
@@ -8240,10 +8294,10 @@
         <v>51</v>
       </c>
       <c r="B341" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C341">
-        <v>76.930999999999997</v>
+        <v>63.569000000000003</v>
       </c>
       <c r="D341" t="s">
         <v>76</v>
@@ -8254,10 +8308,10 @@
         <v>51</v>
       </c>
       <c r="B342" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C342">
-        <v>68.641999999999996</v>
+        <v>76.930999999999997</v>
       </c>
       <c r="D342" t="s">
         <v>76</v>
@@ -8268,10 +8322,10 @@
         <v>51</v>
       </c>
       <c r="B343" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C343">
-        <v>58.533000000000001</v>
+        <v>68.641999999999996</v>
       </c>
       <c r="D343" t="s">
         <v>76</v>
@@ -8279,13 +8333,13 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B344" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C344">
-        <v>90.491</v>
+        <v>58.533000000000001</v>
       </c>
       <c r="D344" t="s">
         <v>76</v>
@@ -8296,10 +8350,10 @@
         <v>52</v>
       </c>
       <c r="B345" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C345">
-        <v>73.566999999999993</v>
+        <v>90.491</v>
       </c>
       <c r="D345" t="s">
         <v>76</v>
@@ -8310,10 +8364,10 @@
         <v>52</v>
       </c>
       <c r="B346" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C346">
-        <v>95.8</v>
+        <v>73.566999999999993</v>
       </c>
       <c r="D346" t="s">
         <v>76</v>
@@ -8324,10 +8378,10 @@
         <v>52</v>
       </c>
       <c r="B347" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C347">
-        <v>87.128</v>
+        <v>95.8</v>
       </c>
       <c r="D347" t="s">
         <v>76</v>
@@ -8338,10 +8392,10 @@
         <v>52</v>
       </c>
       <c r="B348" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C348">
-        <v>76.316000000000003</v>
+        <v>87.128</v>
       </c>
       <c r="D348" t="s">
         <v>76</v>
@@ -8349,13 +8403,13 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B349" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C349">
-        <v>109.85</v>
+        <v>76.316000000000003</v>
       </c>
       <c r="D349" t="s">
         <v>76</v>
@@ -8366,10 +8420,10 @@
         <v>53</v>
       </c>
       <c r="B350" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C350">
-        <v>88.21</v>
+        <v>109.85</v>
       </c>
       <c r="D350" t="s">
         <v>76</v>
@@ -8380,10 +8434,10 @@
         <v>53</v>
       </c>
       <c r="B351" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C351">
-        <v>122.04</v>
+        <v>88.21</v>
       </c>
       <c r="D351" t="s">
         <v>76</v>
@@ -8394,10 +8448,10 @@
         <v>53</v>
       </c>
       <c r="B352" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C352">
-        <v>112.83</v>
+        <v>122.04</v>
       </c>
       <c r="D352" t="s">
         <v>76</v>
@@ -8408,10 +8462,10 @@
         <v>53</v>
       </c>
       <c r="B353" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C353">
-        <v>101.14</v>
+        <v>112.83</v>
       </c>
       <c r="D353" t="s">
         <v>76</v>
@@ -8419,13 +8473,13 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B354" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C354">
-        <v>61.981999999999999</v>
+        <v>101.14</v>
       </c>
       <c r="D354" t="s">
         <v>76</v>
@@ -8436,10 +8490,10 @@
         <v>54</v>
       </c>
       <c r="B355" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C355">
-        <v>24.277000000000001</v>
+        <v>61.981999999999999</v>
       </c>
       <c r="D355" t="s">
         <v>76</v>
@@ -8447,13 +8501,13 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B356" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C356">
-        <v>123.21</v>
+        <v>24.277000000000001</v>
       </c>
       <c r="D356" t="s">
         <v>76</v>
@@ -8464,10 +8518,10 @@
         <v>55</v>
       </c>
       <c r="B357" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C357">
-        <v>44.52</v>
+        <v>123.21</v>
       </c>
       <c r="D357" t="s">
         <v>76</v>
@@ -8475,13 +8529,13 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B358" t="s">
         <v>60</v>
       </c>
       <c r="C358">
-        <v>21.265000000000001</v>
+        <v>44.52</v>
       </c>
       <c r="D358" t="s">
         <v>76</v>
@@ -8489,13 +8543,13 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B359" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C359">
-        <v>75.239000000000004</v>
+        <v>21.265000000000001</v>
       </c>
       <c r="D359" t="s">
         <v>76</v>
@@ -8503,13 +8557,13 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B360" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C360">
-        <v>220.37</v>
+        <v>75.239000000000004</v>
       </c>
       <c r="D360" t="s">
         <v>76</v>
@@ -8517,13 +8571,13 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B361" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C361">
-        <v>102.98</v>
+        <v>220.37</v>
       </c>
       <c r="D361" t="s">
         <v>76</v>
@@ -8534,26 +8588,40 @@
         <v>67</v>
       </c>
       <c r="B362" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C362">
-        <v>568.75</v>
-      </c>
-      <c r="D362">
-        <v>85</v>
+        <v>102.98</v>
+      </c>
+      <c r="D362" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B363" t="s">
         <v>69</v>
       </c>
       <c r="C363">
+        <v>568.75</v>
+      </c>
+      <c r="D363">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>68</v>
+      </c>
+      <c r="B364" t="s">
+        <v>69</v>
+      </c>
+      <c r="C364">
         <v>710.53</v>
       </c>
-      <c r="D363">
+      <c r="D364">
         <v>8</v>
       </c>
     </row>
@@ -8567,7 +8635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>